<commit_message>
All files to scenario1
</commit_message>
<xml_diff>
--- a/Scenario3_savepath/Assets_CPY_input.xlsx
+++ b/Scenario3_savepath/Assets_CPY_input.xlsx
@@ -1,42 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s194463_dtu_dk/Documents/Observation Modeling and Management of Water Sytstems/Assigment/water_resources_model/Scenario3_savepath/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\12345 Obs, Mod and WS Management\2023\WRM_material\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_12D927B012B44B5F69A4CD1E5EF70C3584123CFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D71F12E4-BFE5-0A4C-B644-9A18463BDAE9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="23020" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="6570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -66,6 +54,9 @@
   </si>
   <si>
     <t>Khwae Noi Bamrungdan</t>
+  </si>
+  <si>
+    <t>Kaeng Suea Ten</t>
   </si>
   <si>
     <t>Turbine capacity (MW)</t>
@@ -74,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -431,23 +422,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -455,7 +446,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>4</v>
@@ -467,7 +458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -488,7 +479,7 @@
         <v>13462</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -509,7 +500,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -530,7 +521,7 @@
         <v>9510</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -551,7 +542,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -572,13 +563,26 @@
         <v>939</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="1"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4">
+        <v>48</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>196.88135593220338</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1175</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add excel files to scenarios
</commit_message>
<xml_diff>
--- a/Scenario3_savepath/Assets_CPY_input.xlsx
+++ b/Scenario3_savepath/Assets_CPY_input.xlsx
@@ -1,42 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s194463_dtu_dk/Documents/Observation Modeling and Management of Water Sytstems/Assigment/water_resources_model/Scenario3_savepath/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\12345 Obs, Mod and WS Management\2023\WRM_material\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_12D927B012B44B5F69A4CD1E5EF70C3584123CFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D71F12E4-BFE5-0A4C-B644-9A18463BDAE9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="23020" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="6570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -66,6 +54,9 @@
   </si>
   <si>
     <t>Khwae Noi Bamrungdan</t>
+  </si>
+  <si>
+    <t>Kaeng Suea Ten</t>
   </si>
   <si>
     <t>Turbine capacity (MW)</t>
@@ -74,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -431,23 +422,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -455,7 +446,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>4</v>
@@ -467,7 +458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -488,7 +479,7 @@
         <v>13462</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -509,7 +500,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -530,7 +521,7 @@
         <v>9510</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -551,7 +542,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -572,13 +563,26 @@
         <v>939</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="1"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4">
+        <v>48</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>196.88135593220338</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1175</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>